<commit_message>
Removed frozen panes on incubation tab
And made column for pro_water_body on controlled vocab tab
</commit_message>
<xml_diff>
--- a/Rpkg/inst/extdata/ISRaD_Master_Template.xlsx
+++ b/Rpkg/inst/extdata/ISRaD_Master_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/ISRaD/Rpkg/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shanestoner/Desktop/ISRaD/Rpkg/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB89795D-0B55-4740-B587-A88D7787ED94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A8DBAF-6772-1F45-893E-D0BB0C1E133C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="24640" windowHeight="15100" tabRatio="645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1280" yWindow="700" windowWidth="24640" windowHeight="15100" tabRatio="645" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -6244,8 +6244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q985"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8749,7 +8749,7 @@
   <dimension ref="A1:AZ1502"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:J1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17676,8 +17676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:DJ987"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20781,7 +20781,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>'controlled vocabulary'!$AB$4:$AB$8</xm:f>
@@ -21495,8 +21495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BZ1004"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BC31" sqref="BC31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27373,11 +27373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AG200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="X4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1:AG1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -31643,17 +31640,14 @@
   <mergeCells count="1">
     <mergeCell ref="AU1:AV1"/>
   </mergeCells>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB4" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>INDIRECT(BA4)</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA4" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>$AT$4:$AT$13</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR15" xr:uid="{00000000-0002-0000-0800-000002000000}">
-      <formula1>IF($AQ$15="density",#REF!,IF($AQ$15="particle size",#REF!))</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AS15" xr:uid="{00000000-0002-0000-0800-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR15:AS15" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>IF($AQ$15="density",#REF!,IF($AQ$15="particle size",#REF!))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>